<commit_message>
fixed file with missing col
</commit_message>
<xml_diff>
--- a/html/resources/trialorder/phase2_practice.xlsx
+++ b/html/resources/trialorder/phase2_practice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandradecker/Dropbox/Projects/reactivate/trialorder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F723E53E-B4E0-ED47-B2EF-82D22372B5EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{193DADC7-FF5B-7541-9A23-2F6C571AF05C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-29480" yWindow="3500" windowWidth="27640" windowHeight="16220" xr2:uid="{26530B0F-F0FC-6145-A6AD-C9107C2EF7F0}"/>
   </bookViews>
@@ -429,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78778680-2195-9746-B4E8-AABCCF69AC02}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -442,7 +442,7 @@
     <col min="3" max="3" width="32.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -455,11 +455,11 @@
       <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
+      <c r="F1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -472,11 +472,11 @@
       <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="G2">
+      <c r="F2">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -489,11 +489,11 @@
       <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="G3">
+      <c r="F3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -506,11 +506,11 @@
       <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="G4">
+      <c r="F4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -523,7 +523,7 @@
       <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="G5">
+      <c r="F5">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated phase2 practice removed extra cols
</commit_message>
<xml_diff>
--- a/html/resources/trialorder/phase2_practice.xlsx
+++ b/html/resources/trialorder/phase2_practice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandradecker/Dropbox/Projects/reactivate/trialorder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{193DADC7-FF5B-7541-9A23-2F6C571AF05C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D7C8EE4-B3AA-7F4D-8B8E-DBB65112E978}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-29480" yWindow="3500" windowWidth="27640" windowHeight="16220" xr2:uid="{26530B0F-F0FC-6145-A6AD-C9107C2EF7F0}"/>
   </bookViews>
@@ -429,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78778680-2195-9746-B4E8-AABCCF69AC02}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -442,7 +442,7 @@
     <col min="3" max="3" width="32.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -455,11 +455,11 @@
       <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="E1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -472,11 +472,11 @@
       <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="F2">
+      <c r="E2">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -489,11 +489,11 @@
       <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="F3">
+      <c r="E3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -506,11 +506,11 @@
       <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="F4">
+      <c r="E4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -523,7 +523,7 @@
       <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="F5">
+      <c r="E5">
         <v>3</v>
       </c>
     </row>

</xml_diff>